<commit_message>
add test cases lab4
</commit_message>
<xml_diff>
--- a/lab4/check_list.xlsx
+++ b/lab4/check_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zaptot/Desktop/testing_bsu/lab4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443CE230-0379-5D43-8F80-6615689F8712}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0497959A-1301-A94C-BA6C-FBDC3073DB7A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{B68DBA8B-9BBB-B243-B254-05793203C902}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{B68DBA8B-9BBB-B243-B254-05793203C902}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>тест</t>
   </si>
@@ -69,6 +69,24 @@
   </si>
   <si>
     <t>v1.0</t>
+  </si>
+  <si>
+    <t>Попытка создания проекта при заполнении поля "Описание" невалидным значением</t>
+  </si>
+  <si>
+    <t>Попытка создания проекта с заполнением поля название невалидными символами</t>
+  </si>
+  <si>
+    <t>Попытка создания проекта с заполнением поля Сокращенное название невалидными символами</t>
+  </si>
+  <si>
+    <t>Попытка создания проекта с заполнением поля описание невалидными символами</t>
+  </si>
+  <si>
+    <t>Попытка создания проекта при незаполненом поле "Описание проекта"</t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
 </sst>
 </file>
@@ -78,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -93,8 +111,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +129,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -116,11 +146,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -135,8 +166,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -450,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5923CA5-523B-4442-B309-6225D3FF4D24}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,7 +526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1.2</v>
       </c>
@@ -502,7 +537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1.3</v>
       </c>
@@ -513,7 +548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1.4</v>
       </c>
@@ -524,7 +559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1.5</v>
       </c>
@@ -535,7 +570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1.6</v>
       </c>
@@ -546,25 +581,80 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1.7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1.8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test cases in check list
</commit_message>
<xml_diff>
--- a/lab4/check_list.xlsx
+++ b/lab4/check_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zaptot/Desktop/testing_bsu/lab4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC5747-4EE8-8942-BC81-4C45A6B307F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D4B47D-1A74-C84F-8FCE-9F19C365D2F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{B68DBA8B-9BBB-B243-B254-05793203C902}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>тест</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Проверка правильного отображения задач прикрепленных к этому проекту</t>
+  </si>
+  <si>
+    <t>Проверка отображения полей с большим количеством символов</t>
+  </si>
+  <si>
+    <t>Отображение пустой таблицы</t>
+  </si>
+  <si>
+    <t>отображение большого количества записей</t>
   </si>
 </sst>
 </file>
@@ -494,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5923CA5-523B-4442-B309-6225D3FF4D24}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -700,6 +709,39 @@
         <v>11</v>
       </c>
     </row>
+    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>1.18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1.19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>